<commit_message>
Planilha de resultados consolidada
</commit_message>
<xml_diff>
--- a/results/Metamorphic Tests Results.xlsx
+++ b/results/Metamorphic Tests Results.xlsx
@@ -7,6 +7,7 @@
     <sheet state="visible" name="L2" sheetId="2" r:id="rId6"/>
     <sheet state="visible" name="L3" sheetId="3" r:id="rId7"/>
     <sheet state="visible" name="Agregate Data" sheetId="4" r:id="rId8"/>
+    <sheet state="visible" name="RMs" sheetId="5" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="196">
   <si>
     <t>📊 Level 1 — Scenario 1A</t>
   </si>
@@ -570,6 +571,39 @@
   <si>
     <t>INCONCLUSIVE</t>
   </si>
+  <si>
+    <t>RM</t>
+  </si>
+  <si>
+    <t>TOTAL/RM</t>
+  </si>
+  <si>
+    <t>Additive (A)</t>
+  </si>
+  <si>
+    <t>Exclusive (E)</t>
+  </si>
+  <si>
+    <t>Inclusive (I)</t>
+  </si>
+  <si>
+    <t>Inversive (IV)</t>
+  </si>
+  <si>
+    <t>Boundary (B)</t>
+  </si>
+  <si>
+    <t>Multiplicative (M)</t>
+  </si>
+  <si>
+    <t>Permutative (P)</t>
+  </si>
+  <si>
+    <t>Sustainable (S)</t>
+  </si>
+  <si>
+    <t>TOTAL / LEVEL</t>
+  </si>
 </sst>
 </file>
 
@@ -580,7 +614,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
     <numFmt numFmtId="166" formatCode="m.yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -603,8 +637,13 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -623,6 +662,12 @@
         <bgColor rgb="FFF4C7C3"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF93C47D"/>
+        <bgColor rgb="FF93C47D"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -630,7 +675,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="39">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -718,6 +763,27 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="10" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -808,7 +874,7 @@
       <border/>
     </dxf>
   </dxfs>
-  <tableStyles count="14">
+  <tableStyles count="15">
     <tableStyle count="4" pivot="0" name="L1-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
@@ -889,6 +955,12 @@
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
       <tableStyleElement dxfId="4" size="0" type="wholeTable"/>
     </tableStyle>
+    <tableStyle count="4" pivot="0" name="RMs-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+      <tableStyleElement dxfId="4" size="0" type="wholeTable"/>
+    </tableStyle>
   </tableStyles>
 </styleSheet>
 </file>
@@ -906,6 +978,10 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -996,6 +1072,19 @@
     <tableColumn name="%" id="6"/>
   </tableColumns>
   <tableStyleInfo name="Agregate Data-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:E10" displayName="Tabela_11" name="Tabela_11" id="15">
+  <tableColumns count="5">
+    <tableColumn name="RM" id="1"/>
+    <tableColumn name="L1" id="2"/>
+    <tableColumn name="L2" id="3"/>
+    <tableColumn name="L3" id="4"/>
+    <tableColumn name="TOTAL/RM" id="5"/>
+  </tableColumns>
+  <tableStyleInfo name="RMs-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -26567,7 +26656,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="4" width="12.63"/>
+    <col customWidth="1" min="1" max="1" width="14.75"/>
+    <col customWidth="1" min="2" max="4" width="12.63"/>
     <col customWidth="1" min="5" max="5" width="17.25"/>
     <col customWidth="1" min="6" max="6" width="15.25"/>
   </cols>
@@ -26862,7 +26952,7 @@
       <c r="Z8" s="25"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="25"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="25"/>
       <c r="C9" s="25"/>
       <c r="D9" s="25"/>
@@ -26925,7 +27015,7 @@
       <c r="E11" s="25"/>
       <c r="F11" s="25"/>
       <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
+      <c r="H11" s="32"/>
       <c r="I11" s="25"/>
       <c r="J11" s="25"/>
       <c r="K11" s="25"/>
@@ -26953,8 +27043,8 @@
       <c r="E12" s="25"/>
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
       <c r="J12" s="25"/>
       <c r="K12" s="25"/>
       <c r="L12" s="25"/>
@@ -26981,8 +27071,8 @@
       <c r="E13" s="25"/>
       <c r="F13" s="25"/>
       <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
       <c r="J13" s="25"/>
       <c r="K13" s="25"/>
       <c r="L13" s="25"/>
@@ -33588,4 +33678,207 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="15.13"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="22.5" customHeight="1">
+      <c r="A1" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>176</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" ht="22.5" customHeight="1">
+      <c r="A2" s="33" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="33">
+        <v>0.0</v>
+      </c>
+      <c r="C2" s="33">
+        <v>4.0</v>
+      </c>
+      <c r="D2" s="33">
+        <v>4.0</v>
+      </c>
+      <c r="E2" s="35">
+        <f t="shared" ref="E2:E9" si="1">SUM(B2:D2)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" ht="22.5" customHeight="1">
+      <c r="A3" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="B3" s="33">
+        <v>16.0</v>
+      </c>
+      <c r="C3" s="33">
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="33">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="35">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" ht="22.5" customHeight="1">
+      <c r="A4" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="B4" s="33">
+        <v>0.0</v>
+      </c>
+      <c r="C4" s="33">
+        <v>0.0</v>
+      </c>
+      <c r="D4" s="33">
+        <v>2.0</v>
+      </c>
+      <c r="E4" s="35">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" ht="22.5" customHeight="1">
+      <c r="A5" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" s="33">
+        <v>0.0</v>
+      </c>
+      <c r="C5" s="33">
+        <v>2.0</v>
+      </c>
+      <c r="D5" s="33">
+        <v>4.0</v>
+      </c>
+      <c r="E5" s="35">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" ht="22.5" customHeight="1">
+      <c r="A6" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" s="33">
+        <v>0.0</v>
+      </c>
+      <c r="C6" s="33">
+        <v>0.0</v>
+      </c>
+      <c r="D6" s="33">
+        <v>4.0</v>
+      </c>
+      <c r="E6" s="35">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" ht="22.5" customHeight="1">
+      <c r="A7" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="B7" s="33">
+        <v>8.0</v>
+      </c>
+      <c r="C7" s="33">
+        <v>10.0</v>
+      </c>
+      <c r="D7" s="33">
+        <v>8.0</v>
+      </c>
+      <c r="E7" s="35">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" ht="22.5" customHeight="1">
+      <c r="A8" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="B8" s="33">
+        <v>24.0</v>
+      </c>
+      <c r="C8" s="33">
+        <v>10.0</v>
+      </c>
+      <c r="D8" s="33">
+        <v>0.0</v>
+      </c>
+      <c r="E8" s="35">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" ht="22.5" customHeight="1">
+      <c r="A9" s="33" t="s">
+        <v>194</v>
+      </c>
+      <c r="B9" s="33">
+        <v>8.0</v>
+      </c>
+      <c r="C9" s="33">
+        <v>0.0</v>
+      </c>
+      <c r="D9" s="33">
+        <v>0.0</v>
+      </c>
+      <c r="E9" s="35">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" ht="22.5" customHeight="1">
+      <c r="A10" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="B10" s="37">
+        <f t="shared" ref="B10:D10" si="2">SUM(B2:B9)</f>
+        <v>56</v>
+      </c>
+      <c r="C10" s="37">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="D10" s="37">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="E10" s="38"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>